<commit_message>
Creato 15N_recovery_branches e modificato varie volte i file connessi per il calcolo/scaling delle DM di needles e twigs. ancora provvisori.
</commit_message>
<xml_diff>
--- a/15N_experiment/15N_branches/From_diameters_to_DM_per length.xlsx
+++ b/15N_experiment/15N_branches/From_diameters_to_DM_per length.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>B01</t>
   </si>
@@ -107,13 +107,28 @@
   </si>
   <si>
     <t>Notes: new and old leaves, new and old twigs are predicted by the length_weight.R script in the branches folder in Repo and are expressed in g/cm</t>
+  </si>
+  <si>
+    <t>valore preso spannometricamente sulla curva per eliminare quei valori di tozzy che non rappresentano un diametro verosimile tra I miei diametri campionati</t>
+  </si>
+  <si>
+    <t>valori rapprsentativi della prima parte della curva, quella che contiene tutti I valori dei new twigs pesati in laboratorio</t>
+  </si>
+  <si>
+    <t>valore rapprsentativo della seconda parte della curva, quella che contiene tutti I valori degli old twigs pesati in laboratorio</t>
+  </si>
+  <si>
+    <t>I valori cosi calcolati sono I miei valori di peso riportati su branch_15N</t>
+  </si>
+  <si>
+    <t>ottenuto come valore proporzionale all'old max, ricavato dalla media dei valori pesati old e new (old pesano mediamente 0.40, new 0.18)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,16 +149,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -151,11 +179,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -176,8 +220,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -456,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H11"/>
+      <selection activeCell="C2" sqref="C2:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,16 +526,16 @@
       <c r="D1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="8" t="s">
         <v>19</v>
       </c>
     </row>
@@ -498,24 +547,24 @@
         <v>8.1</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C11" si="0">New_min+(B2-Bmin)/(Bmax-Bmin)*(New_max-New_min)</f>
-        <v>1.7853100333333333E-2</v>
+        <f>New_min+(B2-Bmin)/(Bmax-Bmin)*(New_max-New_min)</f>
+        <v>1.3419766666666666E-2</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D11" si="1">Old_min+(B2-Bmin)/(Bmax-Bmin)*(old_max-Old_min)</f>
-        <v>4.3070075999999999E-2</v>
-      </c>
-      <c r="E2" s="7">
-        <v>4.3776190000000001</v>
-      </c>
-      <c r="F2">
-        <v>10.765530999999999</v>
-      </c>
-      <c r="G2">
-        <v>1.3078299</v>
-      </c>
-      <c r="H2">
-        <v>4.568695</v>
+        <f t="shared" ref="D2:D11" si="0">Old_min+(B2-Bmin)/(Bmax-Bmin)*(old_max-Old_min)</f>
+        <v>2.4217601333333335E-2</v>
+      </c>
+      <c r="E2" s="9">
+        <v>3.6791589999999998</v>
+      </c>
+      <c r="F2" s="8">
+        <v>9.1576050000000002</v>
+      </c>
+      <c r="G2" s="8">
+        <v>1.0898953</v>
+      </c>
+      <c r="H2" s="8">
+        <v>3.2756789999999998</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -526,24 +575,24 @@
         <v>13.8</v>
       </c>
       <c r="C3">
+        <f t="shared" ref="C3:C11" si="1">New_min+(B3-Bmin)/(Bmax-Bmin)*(New_max-New_min)</f>
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="D3">
         <f t="shared" si="0"/>
-        <v>2.9090910000000001E-2</v>
-      </c>
-      <c r="D3">
-        <f t="shared" si="1"/>
-        <v>8.6415839999999994E-2</v>
-      </c>
-      <c r="E3" s="7">
-        <v>9.459028</v>
-      </c>
-      <c r="F3">
-        <v>11.615088</v>
-      </c>
-      <c r="G3">
-        <v>3.4615041999999998</v>
-      </c>
-      <c r="H3">
-        <v>9.8275860000000002</v>
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="E3" s="9">
+        <v>8.2015580000000003</v>
+      </c>
+      <c r="F3" s="8">
+        <v>10.416109909249871</v>
+      </c>
+      <c r="G3" s="8">
+        <v>2.6836712999999999</v>
+      </c>
+      <c r="H3" s="8">
+        <v>5.0278081701978214</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -554,24 +603,24 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="C4">
+        <f t="shared" si="1"/>
+        <v>1.354538888888889E-2</v>
+      </c>
+      <c r="D4">
         <f t="shared" si="0"/>
-        <v>1.8247409444444446E-2</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="1"/>
-        <v>4.4590980000000002E-2</v>
-      </c>
-      <c r="E4" s="7">
-        <v>4.5927129999999998</v>
-      </c>
-      <c r="F4">
-        <v>10.831301</v>
-      </c>
-      <c r="G4">
-        <v>1.3753842000000001</v>
-      </c>
-      <c r="H4">
-        <v>4.6785119999999996</v>
+        <v>2.4595931111111115E-2</v>
+      </c>
+      <c r="E4" s="9">
+        <v>3.7824490000000002</v>
+      </c>
+      <c r="F4" s="8">
+        <v>9.1951970000000003</v>
+      </c>
+      <c r="G4" s="8">
+        <v>1.1136950999999999</v>
+      </c>
+      <c r="H4" s="8">
+        <v>3.3585850000000002</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -582,24 +631,24 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="C5">
+        <f t="shared" si="1"/>
+        <v>1.4110688888888889E-2</v>
+      </c>
+      <c r="D5">
         <f t="shared" si="0"/>
-        <v>2.0021800444444446E-2</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="1"/>
-        <v>5.1435047999999997E-2</v>
-      </c>
-      <c r="E5" s="7">
-        <v>5.6826249999999998</v>
-      </c>
-      <c r="F5">
-        <v>11.056422</v>
-      </c>
-      <c r="G5">
-        <v>1.7279456</v>
-      </c>
-      <c r="H5">
-        <v>5.500102</v>
+        <v>2.6298415111111112E-2</v>
+      </c>
+      <c r="E5" s="9">
+        <v>4.2803560000000003</v>
+      </c>
+      <c r="F5" s="8">
+        <v>9.4975480000000001</v>
+      </c>
+      <c r="G5" s="8">
+        <v>1.2245793</v>
+      </c>
+      <c r="H5" s="8">
+        <v>3.72295</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -610,24 +659,24 @@
         <v>12.2</v>
       </c>
       <c r="C6">
+        <f t="shared" si="1"/>
+        <v>1.5995022222222224E-2</v>
+      </c>
+      <c r="D6">
         <f t="shared" si="0"/>
-        <v>2.5936437111111113E-2</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="1"/>
-        <v>7.4248607999999994E-2</v>
-      </c>
-      <c r="E6" s="7">
-        <v>8.6939869999999999</v>
-      </c>
-      <c r="F6">
-        <v>11.539702999999999</v>
-      </c>
-      <c r="G6">
-        <v>2.9516406000000002</v>
-      </c>
-      <c r="H6">
-        <v>9.2403650000000006</v>
+        <v>3.1973361777777778E-2</v>
+      </c>
+      <c r="E6" s="9">
+        <v>6.8900509999999997</v>
+      </c>
+      <c r="F6" s="8">
+        <v>11.10769</v>
+      </c>
+      <c r="G6" s="8">
+        <v>2.1541255000000001</v>
+      </c>
+      <c r="H6" s="8">
+        <v>4.7273849999999999</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -638,24 +687,24 @@
         <v>10.4</v>
       </c>
       <c r="C7">
+        <f t="shared" si="1"/>
+        <v>1.4864422222222222E-2</v>
+      </c>
+      <c r="D7">
         <f t="shared" si="0"/>
-        <v>2.2387655111111113E-2</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="1"/>
-        <v>6.056047199999999E-2</v>
-      </c>
-      <c r="E7" s="7">
-        <v>7.1709290000000001</v>
-      </c>
-      <c r="F7">
-        <v>11.314959</v>
-      </c>
-      <c r="G7">
-        <v>2.2514297000000001</v>
-      </c>
-      <c r="H7">
-        <v>7.3706750000000003</v>
+        <v>2.8568393777777781E-2</v>
+      </c>
+      <c r="E7" s="9">
+        <v>5.1697930000000003</v>
+      </c>
+      <c r="F7" s="8">
+        <v>10.146962</v>
+      </c>
+      <c r="G7" s="8">
+        <v>1.5206025000000001</v>
+      </c>
+      <c r="H7" s="8">
+        <v>4.1761619999999997</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -666,24 +715,24 @@
         <v>8</v>
       </c>
       <c r="C8">
+        <f t="shared" si="1"/>
+        <v>1.3356955555555557E-2</v>
+      </c>
+      <c r="D8">
         <f t="shared" si="0"/>
-        <v>1.7655945777777779E-2</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="1"/>
-        <v>4.2309623999999997E-2</v>
-      </c>
-      <c r="E8" s="7">
-        <v>4.2754799999999999</v>
-      </c>
-      <c r="F8">
-        <v>10.729081000000001</v>
-      </c>
-      <c r="G8">
-        <v>1.2759606999999999</v>
-      </c>
-      <c r="H8">
-        <v>4.5193370000000002</v>
+        <v>2.4028436444444447E-2</v>
+      </c>
+      <c r="E8" s="9">
+        <v>3.628342</v>
+      </c>
+      <c r="F8" s="8">
+        <v>9.1255269999999999</v>
+      </c>
+      <c r="G8" s="8">
+        <v>1.077523</v>
+      </c>
+      <c r="H8" s="8">
+        <v>3.2321930000000001</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -694,24 +743,24 @@
         <v>4.8</v>
       </c>
       <c r="C9">
+        <f t="shared" si="1"/>
+        <v>1.1346999999999999E-2</v>
+      </c>
+      <c r="D9">
         <f t="shared" si="0"/>
-        <v>1.1346999999999999E-2</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="1"/>
         <v>1.797516E-2</v>
       </c>
-      <c r="E9" s="7">
-        <v>2.5400309999999999</v>
-      </c>
-      <c r="F9">
-        <v>4.4427269999999996</v>
-      </c>
-      <c r="G9">
-        <v>0.84206780000000003</v>
-      </c>
-      <c r="H9">
-        <v>1.3282149999999999</v>
+      <c r="E9" s="9">
+        <v>2.516108</v>
+      </c>
+      <c r="F9" s="8">
+        <v>4.3705759999999998</v>
+      </c>
+      <c r="G9" s="8">
+        <v>0.80937700000000001</v>
+      </c>
+      <c r="H9" s="8">
+        <v>1.2513080000000001</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -722,24 +771,24 @@
         <v>6.1</v>
       </c>
       <c r="C10">
+        <f t="shared" si="1"/>
+        <v>1.2163544444444445E-2</v>
+      </c>
+      <c r="D10">
         <f t="shared" si="0"/>
-        <v>1.3910009222222221E-2</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="1"/>
-        <v>2.7861035999999999E-2</v>
-      </c>
-      <c r="E10" s="7">
-        <v>3.0135550000000002</v>
-      </c>
-      <c r="F10">
-        <v>9.2106580000000005</v>
-      </c>
-      <c r="G10">
-        <v>0.91145319999999996</v>
-      </c>
-      <c r="H10">
-        <v>3.2738960000000001</v>
+        <v>2.0434303555555557E-2</v>
+      </c>
+      <c r="E10" s="9">
+        <v>2.8459840000000001</v>
+      </c>
+      <c r="F10" s="8">
+        <v>6.727004</v>
+      </c>
+      <c r="G10" s="8">
+        <v>0.8950574</v>
+      </c>
+      <c r="H10" s="8">
+        <v>2.0917500000000002</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -750,24 +799,24 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="C11">
+        <f t="shared" si="1"/>
+        <v>1.3796633333333332E-2</v>
+      </c>
+      <c r="D11">
         <f t="shared" si="0"/>
-        <v>1.9036027666666667E-2</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="1"/>
-        <v>4.7632787999999995E-2</v>
-      </c>
-      <c r="E11" s="7">
-        <v>5.0581769999999997</v>
-      </c>
-      <c r="F11">
-        <v>10.940937</v>
-      </c>
-      <c r="G11">
-        <v>1.5237206999999999</v>
-      </c>
-      <c r="H11">
-        <v>4.9629459999999996</v>
+        <v>2.5352590666666668E-2</v>
+      </c>
+      <c r="E11" s="9">
+        <v>3.9957220000000002</v>
+      </c>
+      <c r="F11" s="8">
+        <v>9.3012929999999994</v>
+      </c>
+      <c r="G11" s="8">
+        <v>1.1575108000000001</v>
+      </c>
+      <c r="H11" s="8">
+        <v>3.5221640000000001</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -799,34 +848,57 @@
       <c r="B15">
         <v>1.1346999999999999E-2</v>
       </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B16">
-        <v>2.9090910000000001E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B17">
         <v>1.797516E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B18">
-        <v>8.6415839999999994E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <f>old_max*18/40</f>
+        <v>1.5750000000000004E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Further corrections on 15N recovery on branches and created plots. also needs to calculate the applied 15N properly.
</commit_message>
<xml_diff>
--- a/15N_experiment/15N_branches/From_diameters_to_DM_per length.xlsx
+++ b/15N_experiment/15N_branches/From_diameters_to_DM_per length.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>B01</t>
   </si>
@@ -88,12 +88,6 @@
     <t>diameter</t>
   </si>
   <si>
-    <t>new_twigs</t>
-  </si>
-  <si>
-    <t>old_twigs</t>
-  </si>
-  <si>
     <t>new_leaves</t>
   </si>
   <si>
@@ -122,6 +116,9 @@
   </si>
   <si>
     <t>ottenuto come valore proporzionale all'old max, ricavato dalla media dei valori pesati old e new (old pesano mediamente 0.40, new 0.18)</t>
+  </si>
+  <si>
+    <t>Sto a scoppia', ho cambiato di ogni, non so come cazzo avevo ragionato prima, ma il ragionamento corretto dovrebbe essere: qui mi sono ricalcolato le masse dei rametti partendo dalle pesate/ lunghezze di laboratorio e rapportandoli ai rami trattati (ma in teorira, spero, solo per proporzionarli tra loro all'interno dei valori da laboratorio. Puo' essere che ho fatto una cazzata ad eliminare i lavori di lab piu alti che in effetti dovrebbero rappresentare i rami piu grossi, ma li avevo tolti quando avevo calcolato erroneamente le masse dei rametti con un doppio passaggio concettualmente sbagliato</t>
   </si>
 </sst>
 </file>
@@ -505,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D11"/>
+      <selection activeCell="D2" sqref="D2:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,23 +518,19 @@
         <v>17</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="8" t="s">
         <v>19</v>
       </c>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -548,24 +541,20 @@
       </c>
       <c r="C2">
         <f>New_min+(B2-Bmin)/(Bmax-Bmin)*(New_max-New_min)</f>
-        <v>1.3419766666666666E-2</v>
+        <v>1.7853100333333333E-2</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D11" si="0">Old_min+(B2-Bmin)/(Bmax-Bmin)*(old_max-Old_min)</f>
-        <v>2.4217601333333335E-2</v>
+        <v>4.3070075999999999E-2</v>
       </c>
       <c r="E2" s="9">
-        <v>3.6791589999999998</v>
+        <v>6.421731E-2</v>
       </c>
       <c r="F2" s="8">
-        <v>9.1576050000000002</v>
-      </c>
-      <c r="G2" s="8">
-        <v>1.0898953</v>
-      </c>
-      <c r="H2" s="8">
-        <v>3.2756789999999998</v>
-      </c>
+        <v>0.10140037</v>
+      </c>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -575,25 +564,21 @@
         <v>13.8</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C11" si="1">New_min+(B3-Bmin)/(Bmax-Bmin)*(New_max-New_min)</f>
-        <v>1.7000000000000001E-2</v>
+        <f t="shared" ref="C3:D11" si="1">New_min+(B3-Bmin)/(Bmax-Bmin)*(New_max-New_min)</f>
+        <v>2.9090910000000001E-2</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>3.5000000000000003E-2</v>
+        <v>8.6415839999999994E-2</v>
       </c>
       <c r="E3" s="9">
-        <v>8.2015580000000003</v>
+        <v>7.9206310000000002E-2</v>
       </c>
       <c r="F3" s="8">
-        <v>10.416109909249871</v>
-      </c>
-      <c r="G3" s="8">
-        <v>2.6836712999999999</v>
-      </c>
-      <c r="H3" s="8">
-        <v>5.0278081701978214</v>
-      </c>
+        <v>0.11555194000000001</v>
+      </c>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -604,24 +589,20 @@
       </c>
       <c r="C4">
         <f t="shared" si="1"/>
-        <v>1.354538888888889E-2</v>
+        <v>1.8247409444444446E-2</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>2.4595931111111115E-2</v>
+        <v>4.4590980000000002E-2</v>
       </c>
       <c r="E4" s="9">
-        <v>3.7824490000000002</v>
+        <v>6.5873650000000006E-2</v>
       </c>
       <c r="F4" s="8">
-        <v>9.1951970000000003</v>
-      </c>
-      <c r="G4" s="8">
-        <v>1.1136950999999999</v>
-      </c>
-      <c r="H4" s="8">
-        <v>3.3585850000000002</v>
-      </c>
+        <v>0.10388062000000001</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -632,24 +613,20 @@
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>1.4110688888888889E-2</v>
+        <v>2.0021800444444446E-2</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>2.6298415111111112E-2</v>
+        <v>5.1435047999999997E-2</v>
       </c>
       <c r="E5" s="9">
-        <v>4.2803560000000003</v>
+        <v>7.0001350000000004E-2</v>
       </c>
       <c r="F5" s="8">
-        <v>9.4975480000000001</v>
-      </c>
-      <c r="G5" s="8">
-        <v>1.2245793</v>
-      </c>
-      <c r="H5" s="8">
-        <v>3.72295</v>
-      </c>
+        <v>0.11193648</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -660,24 +637,20 @@
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>1.5995022222222224E-2</v>
+        <v>2.5936437111111113E-2</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>3.1973361777777778E-2</v>
+        <v>7.4248607999999994E-2</v>
       </c>
       <c r="E6" s="9">
-        <v>6.8900509999999997</v>
+        <v>7.6529520000000004E-2</v>
       </c>
       <c r="F6" s="8">
-        <v>11.10769</v>
-      </c>
-      <c r="G6" s="8">
-        <v>2.1541255000000001</v>
-      </c>
-      <c r="H6" s="8">
-        <v>4.7273849999999999</v>
-      </c>
+        <v>0.12051626999999999</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -688,24 +661,20 @@
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>1.4864422222222222E-2</v>
+        <v>2.2387655111111113E-2</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>2.8568393777777781E-2</v>
+        <v>6.056047199999999E-2</v>
       </c>
       <c r="E7" s="9">
-        <v>5.1697930000000003</v>
+        <v>7.2451420000000002E-2</v>
       </c>
       <c r="F7" s="8">
-        <v>10.146962</v>
-      </c>
-      <c r="G7" s="8">
-        <v>1.5206025000000001</v>
-      </c>
-      <c r="H7" s="8">
-        <v>4.1761619999999997</v>
-      </c>
+        <v>0.11830346</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -716,24 +685,20 @@
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>1.3356955555555557E-2</v>
+        <v>1.7655945777777779E-2</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>2.4028436444444447E-2</v>
+        <v>4.2309623999999997E-2</v>
       </c>
       <c r="E8" s="9">
-        <v>3.628342</v>
+        <v>6.3216700000000001E-2</v>
       </c>
       <c r="F8" s="8">
-        <v>9.1255269999999999</v>
-      </c>
-      <c r="G8" s="8">
-        <v>1.077523</v>
-      </c>
-      <c r="H8" s="8">
-        <v>3.2321930000000001</v>
-      </c>
+        <v>0.10009229</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -751,17 +716,13 @@
         <v>1.797516E-2</v>
       </c>
       <c r="E9" s="9">
-        <v>2.516108</v>
+        <v>4.7212379999999998E-2</v>
       </c>
       <c r="F9" s="8">
-        <v>4.3705759999999998</v>
-      </c>
-      <c r="G9" s="8">
-        <v>0.80937700000000001</v>
-      </c>
-      <c r="H9" s="8">
-        <v>1.2513080000000001</v>
-      </c>
+        <v>6.4787600000000001E-2</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -772,24 +733,20 @@
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>1.2163544444444445E-2</v>
+        <v>1.3910009222222221E-2</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>2.0434303555555557E-2</v>
+        <v>2.7861035999999999E-2</v>
       </c>
       <c r="E10" s="9">
-        <v>2.8459840000000001</v>
+        <v>5.0821570000000003E-2</v>
       </c>
       <c r="F10" s="8">
-        <v>6.727004</v>
-      </c>
-      <c r="G10" s="8">
-        <v>0.8950574</v>
-      </c>
-      <c r="H10" s="8">
-        <v>2.0917500000000002</v>
-      </c>
+        <v>7.8284809999999996E-2</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -800,24 +757,20 @@
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>1.3796633333333332E-2</v>
+        <v>1.9036027666666667E-2</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>2.5352590666666668E-2</v>
+        <v>4.7632787999999995E-2</v>
       </c>
       <c r="E11" s="9">
-        <v>3.9957220000000002</v>
+        <v>6.8103419999999998E-2</v>
       </c>
       <c r="F11" s="8">
-        <v>9.3012929999999994</v>
-      </c>
-      <c r="G11" s="8">
-        <v>1.1575108000000001</v>
-      </c>
-      <c r="H11" s="8">
-        <v>3.5221640000000001</v>
-      </c>
+        <v>0.10806316000000001</v>
+      </c>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -849,7 +802,7 @@
         <v>1.1346999999999999E-2</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -857,10 +810,10 @@
         <v>13</v>
       </c>
       <c r="B16">
-        <v>1.7000000000000001E-2</v>
+        <v>2.9090910000000001E-2</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -871,7 +824,7 @@
         <v>1.797516E-2</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -879,26 +832,25 @@
         <v>15</v>
       </c>
       <c r="B18">
-        <v>3.5000000000000003E-2</v>
+        <v>8.6415839999999994E-2</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C26">
-        <f>old_max*18/40</f>
-        <v>1.5750000000000004E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>